<commit_message>
check valid import students to class, add loading
</commit_message>
<xml_diff>
--- a/public/assets/template_import_danh_sach_sinh_vien.xlsx
+++ b/public/assets/template_import_danh_sach_sinh_vien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A! Template KLTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C7E8F9-5628-4F99-9C81-5949B6EFFDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68916A19-3242-4804-B025-AB09F929CEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -746,9 +746,6 @@
     <t>PMCL2021.2</t>
   </si>
   <si>
-    <t>Danh sách lớp PMCL2021.2</t>
-  </si>
-  <si>
     <t>Nữ</t>
   </si>
   <si>
@@ -756,6 +753,9 @@
   </si>
   <si>
     <t>26/09/2003</t>
+  </si>
+  <si>
+    <t>Danh sách sinh viên</t>
   </si>
 </sst>
 </file>
@@ -825,13 +825,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1174,38 +1174,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="28.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" style="2" customWidth="1"/>
-    <col min="5" max="9" width="30.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="19.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="2" customWidth="1"/>
+    <col min="5" max="9" width="30.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="1" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1239,7 +1239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1261,18 +1261,18 @@
       <c r="G3" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>239</v>
+      <c r="H3" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1292,20 +1292,20 @@
         <v>235</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1327,18 +1327,18 @@
       <c r="G5" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>239</v>
+      <c r="H5" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1360,18 +1360,18 @@
       <c r="G6" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>239</v>
+      <c r="H6" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1391,21 +1391,21 @@
         <v>235</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1426,19 +1426,19 @@
       <c r="G8" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>239</v>
+      <c r="H8" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1459,19 +1459,19 @@
       <c r="G9" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>239</v>
+      <c r="H9" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1492,19 +1492,19 @@
       <c r="G10" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>239</v>
+      <c r="H10" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1525,19 +1525,19 @@
       <c r="G11" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>239</v>
+      <c r="H11" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1556,21 +1556,21 @@
         <v>235</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1589,21 +1589,21 @@
         <v>235</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1624,19 +1624,19 @@
       <c r="G14" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>239</v>
+      <c r="H14" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1657,19 +1657,19 @@
       <c r="G15" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>239</v>
+      <c r="H15" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>60</v>
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1690,19 +1690,19 @@
       <c r="G16" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>239</v>
+      <c r="H16" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1723,19 +1723,19 @@
       <c r="G17" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>239</v>
+      <c r="H17" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1756,19 +1756,19 @@
       <c r="G18" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>239</v>
+      <c r="H18" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1789,19 +1789,19 @@
       <c r="G19" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>239</v>
+      <c r="H19" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1822,19 +1822,19 @@
       <c r="G20" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>239</v>
+      <c r="H20" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1853,21 +1853,21 @@
         <v>235</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1888,19 +1888,19 @@
       <c r="G22" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H22" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>239</v>
+      <c r="H22" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1921,19 +1921,19 @@
       <c r="G23" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H23" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>239</v>
+      <c r="H23" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1954,19 +1954,19 @@
       <c r="G24" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H24" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>239</v>
+      <c r="H24" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1987,19 +1987,19 @@
       <c r="G25" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H25" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>239</v>
+      <c r="H25" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2020,19 +2020,19 @@
       <c r="G26" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H26" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>239</v>
+      <c r="H26" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2053,19 +2053,19 @@
       <c r="G27" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H27" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>239</v>
+      <c r="H27" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2086,19 +2086,19 @@
       <c r="G28" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H28" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>239</v>
+      <c r="H28" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2119,19 +2119,19 @@
       <c r="G29" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H29" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>239</v>
+      <c r="H29" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2152,19 +2152,19 @@
       <c r="G30" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H30" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>239</v>
+      <c r="H30" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2185,19 +2185,19 @@
       <c r="G31" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H31" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>239</v>
+      <c r="H31" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2218,19 +2218,19 @@
       <c r="G32" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H32" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>239</v>
+      <c r="H32" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2251,19 +2251,19 @@
       <c r="G33" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H33" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>239</v>
+      <c r="H33" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="8">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2284,19 +2284,19 @@
       <c r="G34" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H34" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>239</v>
+      <c r="H34" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="8">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2317,19 +2317,19 @@
       <c r="G35" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H35" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>239</v>
+      <c r="H35" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>60</v>
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="8">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2350,19 +2350,19 @@
       <c r="G36" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H36" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>239</v>
+      <c r="H36" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="8">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2383,19 +2383,19 @@
       <c r="G37" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H37" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>239</v>
+      <c r="H37" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="8">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2416,19 +2416,19 @@
       <c r="G38" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H38" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>239</v>
+      <c r="H38" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="8">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2449,19 +2449,19 @@
       <c r="G39" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H39" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>239</v>
+      <c r="H39" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>157</v>
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="8">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2482,19 +2482,19 @@
       <c r="G40" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H40" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>239</v>
+      <c r="H40" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="8">
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2515,19 +2515,19 @@
       <c r="G41" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H41" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>239</v>
+      <c r="H41" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="8">
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2548,19 +2548,19 @@
       <c r="G42" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H42" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>239</v>
+      <c r="H42" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="8">
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2581,19 +2581,19 @@
       <c r="G43" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H43" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>239</v>
+      <c r="H43" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="8">
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2614,19 +2614,19 @@
       <c r="G44" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H44" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I44" s="9" t="s">
-        <v>239</v>
+      <c r="H44" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="8">
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2647,19 +2647,19 @@
       <c r="G45" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H45" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>239</v>
+      <c r="H45" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="8">
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2680,19 +2680,19 @@
       <c r="G46" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H46" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I46" s="9" t="s">
-        <v>239</v>
+      <c r="H46" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="8">
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2713,19 +2713,19 @@
       <c r="G47" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H47" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>239</v>
+      <c r="H47" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="8">
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2746,19 +2746,19 @@
       <c r="G48" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H48" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I48" s="9" t="s">
-        <v>239</v>
+      <c r="H48" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>60</v>
       </c>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="8">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2779,19 +2779,19 @@
       <c r="G49" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H49" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I49" s="9" t="s">
-        <v>239</v>
+      <c r="H49" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="8">
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2812,19 +2812,19 @@
       <c r="G50" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H50" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I50" s="9" t="s">
-        <v>239</v>
+      <c r="H50" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="8">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2845,19 +2845,19 @@
       <c r="G51" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H51" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I51" s="9" t="s">
-        <v>239</v>
+      <c r="H51" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="8">
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2878,19 +2878,19 @@
       <c r="G52" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H52" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I52" s="9" t="s">
-        <v>239</v>
+      <c r="H52" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="8">
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2911,19 +2911,19 @@
       <c r="G53" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H53" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I53" s="9" t="s">
-        <v>239</v>
+      <c r="H53" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="8">
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2944,19 +2944,19 @@
       <c r="G54" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H54" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I54" s="9" t="s">
-        <v>239</v>
+      <c r="H54" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="8">
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2977,19 +2977,19 @@
       <c r="G55" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H55" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I55" s="9" t="s">
-        <v>239</v>
+      <c r="H55" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="8">
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -3010,19 +3010,19 @@
       <c r="G56" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H56" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I56" s="9" t="s">
-        <v>239</v>
+      <c r="H56" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="8">
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -3043,11 +3043,11 @@
       <c r="G57" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H57" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I57" s="9" t="s">
-        <v>239</v>
+      <c r="H57" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>11</v>
@@ -3067,6 +3067,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Tài liệu" ma:contentTypeID="0x01010097A8FBAA2E37D445A4C9C7B59250E3D8" ma:contentTypeVersion="8" ma:contentTypeDescription="Tạo tài liệu mới." ma:contentTypeScope="" ma:versionID="d6a65ad03dfb631e1e1453bcf9fdce07">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d78d4705-7cc3-4b19-ac87-7faa7a5222da" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="da17fd8323a344df5d8056072407b4d4" ns2:_="">
     <xsd:import namespace="d78d4705-7cc3-4b19-ac87-7faa7a5222da"/>
@@ -3234,16 +3243,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA8E4CE1-20B2-494C-9DBB-3146660364FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1340B7FB-D452-41B3-A987-66862BF3DCB3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3259,12 +3267,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA8E4CE1-20B2-494C-9DBB-3146660364FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>